<commit_message>
changed the exel format
</commit_message>
<xml_diff>
--- a/excel/2006-01-02.xlsx
+++ b/excel/2006-01-02.xlsx
@@ -69,7 +69,7 @@
     <t>業主</t>
   </si>
   <si>
-    <t>11426</t>
+    <t>1140206</t>
   </si>
   <si>
     <t>KEQ8006</t>
@@ -81,16 +81,16 @@
     <t/>
   </si>
   <si>
-    <t>11428</t>
-  </si>
-  <si>
-    <t>114224</t>
-  </si>
-  <si>
-    <t>114228</t>
-  </si>
-  <si>
-    <t>11431</t>
+    <t>1140208</t>
+  </si>
+  <si>
+    <t>1140224</t>
+  </si>
+  <si>
+    <t>1140228</t>
+  </si>
+  <si>
+    <t>1140301</t>
   </si>
   <si>
     <t>戲曲</t>
@@ -105,37 +105,37 @@
     <t>永豐哥</t>
   </si>
   <si>
-    <t>11432</t>
-  </si>
-  <si>
-    <t>11433</t>
+    <t>1140302</t>
+  </si>
+  <si>
+    <t>1140303</t>
   </si>
   <si>
     <t>玉成段</t>
   </si>
   <si>
-    <t>11434</t>
-  </si>
-  <si>
-    <t>11435</t>
-  </si>
-  <si>
-    <t>11436</t>
+    <t>1140304</t>
+  </si>
+  <si>
+    <t>1140305</t>
+  </si>
+  <si>
+    <t>1140306</t>
   </si>
   <si>
     <t>大龍</t>
   </si>
   <si>
-    <t>11437</t>
-  </si>
-  <si>
-    <t>11438</t>
-  </si>
-  <si>
-    <t>114310</t>
-  </si>
-  <si>
-    <t>114311</t>
+    <t>1140307</t>
+  </si>
+  <si>
+    <t>1140308</t>
+  </si>
+  <si>
+    <t>1140310</t>
+  </si>
+  <si>
+    <t>1140311</t>
   </si>
   <si>
     <t>南港調車場2</t>
@@ -150,7 +150,7 @@
     <t>林李勝</t>
   </si>
   <si>
-    <t>11425</t>
+    <t>1140205</t>
   </si>
   <si>
     <t>KEP0171</t>
@@ -159,10 +159,10 @@
     <t>王登翊</t>
   </si>
   <si>
-    <t>114218</t>
-  </si>
-  <si>
-    <t>114226</t>
+    <t>1140218</t>
+  </si>
+  <si>
+    <t>1140226</t>
   </si>
   <si>
     <t>辛亥段</t>
@@ -174,10 +174,10 @@
     <t>張浩宇</t>
   </si>
   <si>
-    <t>11427</t>
-  </si>
-  <si>
-    <t>114312</t>
+    <t>1140207</t>
+  </si>
+  <si>
+    <t>1140312</t>
   </si>
   <si>
     <t>KEA0379</t>
@@ -204,7 +204,7 @@
     <t>張國祥</t>
   </si>
   <si>
-    <t>11439</t>
+    <t>1140309</t>
   </si>
   <si>
     <t>學府路</t>
@@ -219,7 +219,7 @@
     <t>阿受</t>
   </si>
   <si>
-    <t>114315</t>
+    <t>1140315</t>
   </si>
   <si>
     <t>應收款總和</t>

</xml_diff>